<commit_message>
fix(reports): Experimental study PDF
</commit_message>
<xml_diff>
--- a/Ring-like_Clustering_Experimental_Study.xlsx
+++ b/Ring-like_Clustering_Experimental_Study.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mella\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mella\OneDrive\Escritorio\ring-clustering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB4F145-8A1C-407D-B0D4-34927CB02BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED05F9EB-D9CF-480F-A36F-7A665B94C8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6350A1ED-2F70-43BA-B277-357BF2BBBD8A}"/>
   </bookViews>
@@ -476,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FE4A33-17AC-4017-B98A-EAF02126E178}">
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -490,7 +490,7 @@
     <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -507,7 +507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -524,17 +524,8 @@
         <f>(C2  + (1 - (D2 - 1)/9)) / 2</f>
         <v>0.16500000000000001</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -548,26 +539,11 @@
         <v>6</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E66" si="0">(C3  + (1 - (D3 - 1)/9)) / 2</f>
+        <f t="shared" ref="E3:E18" si="0">(C3  + (1 - (D3 - 1)/9)) / 2</f>
         <v>0.38722222222222225</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="3">
-        <f>(C2+C3+C4+C5+C6+C20+C21+C22+C23+C24+C38+C39+C40+C41+C42+C56+C57+C58+C59+C60+C74+C75+C76+C78+C77)*100/25</f>
-        <v>33.74666666666667</v>
-      </c>
-      <c r="I3" s="2">
-        <f>(D7+D25+D43+D61+D79)/5</f>
-        <v>5.8400000000000007</v>
-      </c>
-      <c r="J3" s="2">
-        <f>(H3/100 + (1 - (I3 - 1)/9)) / 2</f>
-        <v>0.39984444444444439</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -584,23 +560,8 @@
         <f t="shared" si="0"/>
         <v>0.44277777777777783</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="3">
-        <f>(C8+C9+C10+C11+C12+C26+C27+C28+C29+C30+C44+C45+C46+C47+C48+C62+C63+C64+C65+C66+C80+C81+C82+C83+C84)*100/25</f>
-        <v>37.080000000000005</v>
-      </c>
-      <c r="I4" s="2">
-        <f>(D13+D31+D49+D85+D67)/5</f>
-        <v>5.7200000000000006</v>
-      </c>
-      <c r="J4" s="2">
-        <f t="shared" ref="J4:J5" si="1">(H4/100 + (1 - (I4 - 1)/9)) / 2</f>
-        <v>0.42317777777777776</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -617,23 +578,8 @@
         <f t="shared" si="0"/>
         <v>0.27777777777777779</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="3">
-        <f>(C14+C15+C16+C17+C18+C32+C34+C33+C35+C36+C50+C51+C52+C53+C54+C68+C69+C70+C71+C72+C86+C87+C88+C89+C90)*100/25</f>
-        <v>78.280000000000015</v>
-      </c>
-      <c r="I5" s="2">
-        <f>(D19+D55+D37+D73+D91)/5</f>
-        <v>4.9599999999999991</v>
-      </c>
-      <c r="J5" s="2">
-        <f t="shared" si="1"/>
-        <v>0.67140000000000011</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -651,7 +597,7 @@
         <v>0.49833333333333341</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -663,7 +609,7 @@
         <v>0.26400000000000001</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" ref="D7:E7" si="2">(D2+D3+D4+D5+D6)/5</f>
+        <f t="shared" ref="D7" si="1">(D2+D3+D4+D5+D6)/5</f>
         <v>6</v>
       </c>
       <c r="E7" s="3">
@@ -671,7 +617,7 @@
         <v>0.35422222222222227</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -689,7 +635,7 @@
         <v>0.27777777777777779</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -707,7 +653,7 @@
         <v>0.33166666666666667</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -725,7 +671,7 @@
         <v>0.55222222222222217</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -743,7 +689,7 @@
         <v>0.3855555555555556</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -761,7 +707,7 @@
         <v>0.44277777777777783</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -773,7 +719,7 @@
         <v>0.39600000000000002</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" ref="D13" si="3">(D8+D9+D10+D11+D12)/5</f>
+        <f t="shared" ref="D13" si="2">(D8+D9+D10+D11+D12)/5</f>
         <v>6.4</v>
       </c>
       <c r="E13" s="3">
@@ -781,7 +727,7 @@
         <v>0.39800000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -799,7 +745,7 @@
         <v>0.60777777777777775</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -817,7 +763,7 @@
         <v>0.61111111111111116</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -883,7 +829,7 @@
         <v>0.79800000000000004</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" ref="D19:E19" si="4">(D14+D15+D16+D17+D18)/5</f>
+        <f t="shared" ref="D19" si="3">(D14+D15+D16+D17+D18)/5</f>
         <v>6.4</v>
       </c>
       <c r="E19" s="3">
@@ -993,7 +939,7 @@
         <v>0.46200000000000002</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" ref="D25:E25" si="5">(D20+D21+D22+D23+D24)/5</f>
+        <f t="shared" ref="D25" si="4">(D20+D21+D22+D23+D24)/5</f>
         <v>6.2</v>
       </c>
       <c r="E25" s="3">
@@ -1103,7 +1049,7 @@
         <v>0.59599999999999997</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" ref="D31:E31" si="6">(D26+D27+D28+D29+D30)/5</f>
+        <f t="shared" ref="D31" si="5">(D26+D27+D28+D29+D30)/5</f>
         <v>6.6</v>
       </c>
       <c r="E31" s="3">
@@ -1213,7 +1159,7 @@
         <v>0.79600000000000004</v>
       </c>
       <c r="D37" s="2">
-        <f t="shared" ref="D37:E37" si="7">(D32+D33+D34+D35+D36)/5</f>
+        <f t="shared" ref="D37" si="6">(D32+D33+D34+D35+D36)/5</f>
         <v>4</v>
       </c>
       <c r="E37" s="3">
@@ -1323,7 +1269,7 @@
         <v>0.16733333333333333</v>
       </c>
       <c r="D43" s="2">
-        <f t="shared" ref="D43:E43" si="8">(D38+D39+D40+D41+D42)/5</f>
+        <f t="shared" ref="D43" si="7">(D38+D39+D40+D41+D42)/5</f>
         <v>5.4</v>
       </c>
       <c r="E43" s="3">
@@ -1433,7 +1379,7 @@
         <v>0.26800000000000002</v>
       </c>
       <c r="D49" s="2">
-        <f t="shared" ref="D49:E49" si="9">(D44+D45+D46+D47+D48)/5</f>
+        <f t="shared" ref="D49" si="8">(D44+D45+D46+D47+D48)/5</f>
         <v>5</v>
       </c>
       <c r="E49" s="3">
@@ -1543,7 +1489,7 @@
         <v>0.66</v>
       </c>
       <c r="D55" s="2">
-        <f t="shared" ref="D55:E55" si="10">(D50+D51+D52+D53+D54)/5</f>
+        <f t="shared" ref="D55" si="9">(D50+D51+D52+D53+D54)/5</f>
         <v>6</v>
       </c>
       <c r="E55" s="3">
@@ -1653,7 +1599,7 @@
         <v>0.46400000000000008</v>
       </c>
       <c r="D61" s="2">
-        <f t="shared" ref="D61:E61" si="11">(D56+D57+D58+D59+D60)/5</f>
+        <f t="shared" ref="D61" si="10">(D56+D57+D58+D59+D60)/5</f>
         <v>5</v>
       </c>
       <c r="E61" s="3">
@@ -1763,7 +1709,7 @@
         <v>0.19800000000000001</v>
       </c>
       <c r="D67" s="2">
-        <f t="shared" ref="D67:E67" si="12">(D62+D63+D64+D65+D66)/5</f>
+        <f t="shared" ref="D67" si="11">(D62+D63+D64+D65+D66)/5</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="E67" s="3">
@@ -1873,7 +1819,7 @@
         <v>1</v>
       </c>
       <c r="D73" s="2">
-        <f t="shared" ref="D73:E73" si="13">(D68+D69+D70+D71+D72)/5</f>
+        <f t="shared" ref="D73" si="12">(D68+D69+D70+D71+D72)/5</f>
         <v>3</v>
       </c>
       <c r="E73" s="3">
@@ -1983,7 +1929,7 @@
         <v>0.33</v>
       </c>
       <c r="D79" s="2">
-        <f t="shared" ref="D79:E79" si="14">(D74+D75+D76+D77+D78)/5</f>
+        <f t="shared" ref="D79" si="13">(D74+D75+D76+D77+D78)/5</f>
         <v>6.6</v>
       </c>
       <c r="E79" s="3">
@@ -2093,7 +2039,7 @@
         <v>0.39600000000000002</v>
       </c>
       <c r="D85" s="2">
-        <f t="shared" ref="D85:E85" si="15">(D80+D81+D82+D83+D84)/5</f>
+        <f t="shared" ref="D85" si="14">(D80+D81+D82+D83+D84)/5</f>
         <v>6.2</v>
       </c>
       <c r="E85" s="3">
@@ -2203,12 +2149,74 @@
         <v>0.66</v>
       </c>
       <c r="D91" s="2">
-        <f t="shared" ref="D91:E91" si="16">(D86+D87+D88+D89+D90)/5</f>
+        <f t="shared" ref="D91" si="15">(D86+D87+D88+D89+D90)/5</f>
         <v>5.4</v>
       </c>
       <c r="E91" s="3">
         <f>(E86+E87+E88+E89+E90)/5</f>
         <v>0.58555555555555561</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C94" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B95" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95" s="3">
+        <f>(C2+C3+C4+C5+C6+C20+C21+C22+C23+C24+C38+C39+C40+C41+C42+C56+C57+C58+C59+C60+C74+C75+C76+C78+C77)*100/25</f>
+        <v>33.74666666666667</v>
+      </c>
+      <c r="D95" s="2">
+        <f>(D7+D25+D43+D61+D79)/5</f>
+        <v>5.8400000000000007</v>
+      </c>
+      <c r="E95" s="2">
+        <f>(C95/100 + (1 - (D95 - 1)/9)) / 2</f>
+        <v>0.39984444444444439</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B96" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" s="3">
+        <f>(C8+C9+C10+C11+C12+C26+C27+C28+C29+C30+C44+C45+C46+C47+C48+C62+C63+C64+C65+C66+C80+C81+C82+C83+C84)*100/25</f>
+        <v>37.080000000000005</v>
+      </c>
+      <c r="D96" s="2">
+        <f>(D13+D31+D49+D85+D67)/5</f>
+        <v>5.7200000000000006</v>
+      </c>
+      <c r="E96" s="2">
+        <f t="shared" ref="E96:E97" si="16">(C96/100 + (1 - (D96 - 1)/9)) / 2</f>
+        <v>0.42317777777777776</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B97" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" s="3">
+        <f>(C14+C15+C16+C17+C18+C32+C34+C33+C35+C36+C50+C51+C52+C53+C54+C68+C69+C70+C71+C72+C86+C87+C88+C89+C90)*100/25</f>
+        <v>78.280000000000015</v>
+      </c>
+      <c r="D97" s="2">
+        <f>(D19+D55+D37+D73+D91)/5</f>
+        <v>4.9599999999999991</v>
+      </c>
+      <c r="E97" s="2">
+        <f t="shared" si="16"/>
+        <v>0.67140000000000011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>